<commit_message>
Fix a bug which application can't modify the last record for each employee
</commit_message>
<xml_diff>
--- a/psPunchInfo/punchInOut.xlsx
+++ b/psPunchInfo/punchInOut.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3044" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3022" uniqueCount="351">
   <si>
     <t>Branch</t>
   </si>
@@ -1991,7 +1991,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" ht="18" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" ht="18" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="1" t="s">
@@ -2000,8 +2000,8 @@
       <c r="D22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>14</v>
+      <c r="E22" s="1">
+        <v>1</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>35</v>
@@ -2014,6 +2014,9 @@
       </c>
       <c r="I22" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="J22" s="2">
+        <f>I23-I22</f>
       </c>
     </row>
     <row r="23" ht="18" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2575,7 +2578,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" ht="18" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" ht="18" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
@@ -2584,8 +2587,8 @@
       <c r="D44" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>14</v>
+      <c r="E44" s="1">
+        <v>1</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>35</v>
@@ -2598,6 +2601,9 @@
       </c>
       <c r="I44" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="J44" s="2">
+        <f>I45-I44</f>
       </c>
     </row>
     <row r="45" ht="18" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3106,7 +3112,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="64" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" ht="36" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1" t="s">
@@ -3115,8 +3121,8 @@
       <c r="D64" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E64" s="1" t="s">
-        <v>14</v>
+      <c r="E64" s="1">
+        <v>1</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>35</v>
@@ -3129,6 +3135,9 @@
       </c>
       <c r="I64" s="1" t="s">
         <v>61</v>
+      </c>
+      <c r="J64" s="2">
+        <f>I65-I64</f>
       </c>
     </row>
     <row r="65" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3787,7 +3796,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="90" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" ht="36" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1" t="s">
@@ -3796,8 +3805,8 @@
       <c r="D90" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E90" s="1" t="s">
-        <v>14</v>
+      <c r="E90" s="1">
+        <v>1</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>35</v>
@@ -3810,6 +3819,9 @@
       </c>
       <c r="I90" s="1" t="s">
         <v>77</v>
+      </c>
+      <c r="J90" s="2">
+        <f>I92-I90</f>
       </c>
     </row>
     <row r="91" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -4421,7 +4433,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="114" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" ht="36" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1" t="s">
@@ -4430,8 +4442,8 @@
       <c r="D114" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E114" s="1" t="s">
-        <v>14</v>
+      <c r="E114" s="1">
+        <v>1</v>
       </c>
       <c r="F114" s="1" t="s">
         <v>35</v>
@@ -4444,6 +4456,9 @@
       </c>
       <c r="I114" s="1" t="s">
         <v>111</v>
+      </c>
+      <c r="J114" s="2">
+        <f>I115-I114</f>
       </c>
     </row>
     <row r="115" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -4765,7 +4780,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="127" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" ht="36" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1" t="s">
@@ -4774,8 +4789,8 @@
       <c r="D127" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E127" s="1" t="s">
-        <v>14</v>
+      <c r="E127" s="1">
+        <v>1</v>
       </c>
       <c r="F127" s="1" t="s">
         <v>35</v>
@@ -4788,6 +4803,9 @@
       </c>
       <c r="I127" s="1" t="s">
         <v>125</v>
+      </c>
+      <c r="J127" s="2">
+        <f>I128-I127</f>
       </c>
     </row>
     <row r="128" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -5371,7 +5389,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="150" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" ht="36" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1" t="s">
@@ -5380,8 +5398,8 @@
       <c r="D150" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E150" s="1" t="s">
-        <v>14</v>
+      <c r="E150" s="1">
+        <v>1</v>
       </c>
       <c r="F150" s="1" t="s">
         <v>35</v>
@@ -5394,6 +5412,9 @@
       </c>
       <c r="I150" s="1" t="s">
         <v>146</v>
+      </c>
+      <c r="J150" s="2">
+        <f>I151-I150</f>
       </c>
     </row>
     <row r="151" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -5821,7 +5842,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="167" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" ht="36" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1" t="s">
@@ -5830,8 +5851,8 @@
       <c r="D167" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E167" s="1" t="s">
-        <v>14</v>
+      <c r="E167" s="1">
+        <v>1</v>
       </c>
       <c r="F167" s="1" t="s">
         <v>35</v>
@@ -5844,6 +5865,9 @@
       </c>
       <c r="I167" s="1" t="s">
         <v>161</v>
+      </c>
+      <c r="J167" s="2">
+        <f>I168-I167</f>
       </c>
     </row>
     <row r="168" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6299,7 +6323,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="185" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" ht="36" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1" t="s">
@@ -6308,8 +6332,8 @@
       <c r="D185" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E185" s="1" t="s">
-        <v>14</v>
+      <c r="E185" s="1">
+        <v>1</v>
       </c>
       <c r="F185" s="1" t="s">
         <v>35</v>
@@ -6322,6 +6346,9 @@
       </c>
       <c r="I185" s="1" t="s">
         <v>177</v>
+      </c>
+      <c r="J185" s="2">
+        <f>I186-I185</f>
       </c>
     </row>
     <row r="186" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6883,7 +6910,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="207" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="207" ht="36" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="1"/>
       <c r="B207" s="1"/>
       <c r="C207" s="1" t="s">
@@ -6892,8 +6919,8 @@
       <c r="D207" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E207" s="1" t="s">
-        <v>14</v>
+      <c r="E207" s="1">
+        <v>1</v>
       </c>
       <c r="F207" s="1" t="s">
         <v>35</v>
@@ -6906,6 +6933,9 @@
       </c>
       <c r="I207" s="1" t="s">
         <v>192</v>
+      </c>
+      <c r="J207" s="2">
+        <f>I208-I207</f>
       </c>
     </row>
     <row r="208" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -7414,7 +7444,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="227" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="227" ht="36" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" s="1"/>
       <c r="B227" s="1"/>
       <c r="C227" s="1" t="s">
@@ -7423,8 +7453,8 @@
       <c r="D227" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="E227" s="1" t="s">
-        <v>14</v>
+      <c r="E227" s="1">
+        <v>1</v>
       </c>
       <c r="F227" s="1" t="s">
         <v>35</v>
@@ -7437,6 +7467,9 @@
       </c>
       <c r="I227" s="1" t="s">
         <v>210</v>
+      </c>
+      <c r="J227" s="2">
+        <f>I228-I227</f>
       </c>
     </row>
     <row r="228" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -8020,7 +8053,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="250" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="250" ht="36" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A250" s="1"/>
       <c r="B250" s="1"/>
       <c r="C250" s="1" t="s">
@@ -8029,8 +8062,8 @@
       <c r="D250" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="E250" s="1" t="s">
-        <v>14</v>
+      <c r="E250" s="1">
+        <v>1</v>
       </c>
       <c r="F250" s="1" t="s">
         <v>34</v>
@@ -8043,6 +8076,9 @@
       </c>
       <c r="I250" s="1" t="s">
         <v>228</v>
+      </c>
+      <c r="J250" s="2">
+        <f>I251-I250</f>
       </c>
     </row>
     <row r="251" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -8339,7 +8375,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="262" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="262" ht="36" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" s="1"/>
       <c r="B262" s="1"/>
       <c r="C262" s="1" t="s">
@@ -8348,8 +8384,8 @@
       <c r="D262" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="E262" s="1" t="s">
-        <v>14</v>
+      <c r="E262" s="1">
+        <v>1</v>
       </c>
       <c r="F262" s="1" t="s">
         <v>30</v>
@@ -8362,6 +8398,9 @@
       </c>
       <c r="I262" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="J262" s="2">
+        <f>I263-I262</f>
       </c>
     </row>
     <row r="263" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -8870,7 +8909,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="282" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="282" ht="36" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A282" s="1"/>
       <c r="B282" s="1"/>
       <c r="C282" s="1" t="s">
@@ -8879,8 +8918,8 @@
       <c r="D282" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="E282" s="1" t="s">
-        <v>14</v>
+      <c r="E282" s="1">
+        <v>1</v>
       </c>
       <c r="F282" s="1" t="s">
         <v>35</v>
@@ -8893,6 +8932,9 @@
       </c>
       <c r="I282" s="1" t="s">
         <v>123</v>
+      </c>
+      <c r="J282" s="2">
+        <f>I283-I282</f>
       </c>
     </row>
     <row r="283" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -9479,7 +9521,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="305" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="305" ht="36" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A305" s="1"/>
       <c r="B305" s="1"/>
       <c r="C305" s="1" t="s">
@@ -9488,8 +9530,8 @@
       <c r="D305" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="E305" s="1" t="s">
-        <v>14</v>
+      <c r="E305" s="1">
+        <v>1</v>
       </c>
       <c r="F305" s="1" t="s">
         <v>35</v>
@@ -9502,6 +9544,9 @@
       </c>
       <c r="I305" s="1" t="s">
         <v>270</v>
+      </c>
+      <c r="J305" s="2">
+        <f>I306-I305</f>
       </c>
     </row>
     <row r="306" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -10063,7 +10108,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="327" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="327" ht="36" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A327" s="1"/>
       <c r="B327" s="1"/>
       <c r="C327" s="1" t="s">
@@ -10072,8 +10117,8 @@
       <c r="D327" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="E327" s="1" t="s">
-        <v>14</v>
+      <c r="E327" s="1">
+        <v>1</v>
       </c>
       <c r="F327" s="1" t="s">
         <v>35</v>
@@ -10086,6 +10131,9 @@
       </c>
       <c r="I327" s="1" t="s">
         <v>49</v>
+      </c>
+      <c r="J327" s="2">
+        <f>I328-I327</f>
       </c>
     </row>
     <row r="328" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -10594,7 +10642,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="347" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="347" ht="36" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A347" s="1"/>
       <c r="B347" s="1"/>
       <c r="C347" s="1" t="s">
@@ -10603,8 +10651,8 @@
       <c r="D347" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="E347" s="1" t="s">
-        <v>14</v>
+      <c r="E347" s="1">
+        <v>1</v>
       </c>
       <c r="F347" s="1" t="s">
         <v>34</v>
@@ -10617,6 +10665,9 @@
       </c>
       <c r="I347" s="1" t="s">
         <v>296</v>
+      </c>
+      <c r="J347" s="2">
+        <f>I348-I347</f>
       </c>
     </row>
     <row r="348" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -11200,7 +11251,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="370" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="370" ht="36" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A370" s="1"/>
       <c r="B370" s="1"/>
       <c r="C370" s="1" t="s">
@@ -11209,8 +11260,8 @@
       <c r="D370" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="E370" s="1" t="s">
-        <v>14</v>
+      <c r="E370" s="1">
+        <v>1</v>
       </c>
       <c r="F370" s="1" t="s">
         <v>35</v>
@@ -11223,6 +11274,9 @@
       </c>
       <c r="I370" s="1" t="s">
         <v>125</v>
+      </c>
+      <c r="J370" s="2">
+        <f>I371-I370</f>
       </c>
     </row>
     <row r="371" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -11756,7 +11810,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="391" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="391" ht="36" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A391" s="1"/>
       <c r="B391" s="1"/>
       <c r="C391" s="1" t="s">
@@ -11765,8 +11819,8 @@
       <c r="D391" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="E391" s="1" t="s">
-        <v>14</v>
+      <c r="E391" s="1">
+        <v>1</v>
       </c>
       <c r="F391" s="1" t="s">
         <v>34</v>
@@ -11779,6 +11833,9 @@
       </c>
       <c r="I391" s="1" t="s">
         <v>323</v>
+      </c>
+      <c r="J391" s="2">
+        <f>I392-I391</f>
       </c>
     </row>
     <row r="392" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -12259,7 +12316,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="410" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="410" ht="36" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A410" s="1"/>
       <c r="B410" s="1"/>
       <c r="C410" s="1" t="s">
@@ -12268,8 +12325,8 @@
       <c r="D410" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="E410" s="1" t="s">
-        <v>14</v>
+      <c r="E410" s="1">
+        <v>1</v>
       </c>
       <c r="F410" s="1" t="s">
         <v>34</v>
@@ -12282,6 +12339,9 @@
       </c>
       <c r="I410" s="1" t="s">
         <v>333</v>
+      </c>
+      <c r="J410" s="2">
+        <f>I411-I410</f>
       </c>
     </row>
     <row r="411" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -12868,7 +12928,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="433" ht="18" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="433" ht="18" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A433" s="1"/>
       <c r="B433" s="1"/>
       <c r="C433" s="1" t="s">
@@ -12877,8 +12937,8 @@
       <c r="D433" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="E433" s="1" t="s">
-        <v>14</v>
+      <c r="E433" s="1">
+        <v>1</v>
       </c>
       <c r="F433" s="1" t="s">
         <v>35</v>
@@ -12891,6 +12951,9 @@
       </c>
       <c r="I433" s="1" t="s">
         <v>339</v>
+      </c>
+      <c r="J433" s="2">
+        <f>I434-I433</f>
       </c>
     </row>
     <row r="434" ht="18" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -13452,7 +13515,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="455" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="455" ht="36" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A455" s="1"/>
       <c r="B455" s="1"/>
       <c r="C455" s="1" t="s">
@@ -13461,8 +13524,8 @@
       <c r="D455" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="E455" s="1" t="s">
-        <v>14</v>
+      <c r="E455" s="1">
+        <v>1</v>
       </c>
       <c r="F455" s="1" t="s">
         <v>35</v>
@@ -13475,6 +13538,9 @@
       </c>
       <c r="I455" s="1" t="s">
         <v>348</v>
+      </c>
+      <c r="J455" s="2">
+        <f>I456-I455</f>
       </c>
     </row>
     <row r="456" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Can't use color filling feature, it will crash the xlsx file
</commit_message>
<xml_diff>
--- a/psPunchInfo/punchInOut.xlsx
+++ b/psPunchInfo/punchInOut.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11310"/>
+    <workbookView xWindow="360" yWindow="270" windowWidth="14940" windowHeight="9150"/>
   </bookViews>
   <sheets>
     <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
@@ -1152,10 +1152,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="FFFFFF"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="000000"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1413,10 +1413,10 @@
   <dimension ref="A1:J456"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="B455" sqref="B455"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="44" customWidth="1"/>

</xml_diff>